<commit_message>
updated with last comments
</commit_message>
<xml_diff>
--- a/session02/BackpropagationInExcel.xlsx
+++ b/session02/BackpropagationInExcel.xlsx
@@ -8,22 +8,19 @@
   </bookViews>
   <sheets>
     <sheet name="Backpropagation in PLay" sheetId="4" r:id="rId1"/>
+    <sheet name="Learning rate Plot" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="97">
   <si>
     <t>Assumption :</t>
   </si>
   <si>
     <t>No Bias exists</t>
-  </si>
-  <si>
-    <t>Objective :</t>
   </si>
   <si>
     <t xml:space="preserve">To understand backpropagation and chain rule </t>
@@ -186,9 +183,6 @@
     <t>learning rate</t>
   </si>
   <si>
-    <t>here we did frwd propogation</t>
-  </si>
-  <si>
     <t>δE_total/δw5 = δ(E1 +E2)/δw5 = δ(E1)/δw5 = (δE1/δa_o1) * (δa_o1/δo1) * (δo1/δw5)</t>
   </si>
   <si>
@@ -199,9 +193,6 @@
   </si>
   <si>
     <t>now breaking indivif=dals</t>
-  </si>
-  <si>
-    <t>δE1/δa_o1 = δ(½ * ( t1 - a_o1)²) = (t1 - a_o1) * (-1) = a_o1 - t1</t>
   </si>
   <si>
     <t>substituting E1 and then taking derivative</t>
@@ -335,9 +326,6 @@
   </si>
   <si>
     <t>relationship of E_total wrt w1:</t>
-  </si>
-  <si>
-    <t>δE_total/δw1 = δ(E_total)/δa_o1 * δa_o1/δo1 * δo1/δa_h1 * δa_h1/δh1 * δh1/δw1</t>
   </si>
   <si>
     <t>δE_total/δw1 = δ(E_total)/δa_h1 * δa_h1/δh1 * δh1/δw1</t>
@@ -531,6 +519,65 @@
   <si>
     <t>=( (a_o1 - t1) * a_o1 * (1 - a_o1 ) * w5 + (a_o2 - t2) * a_o2 * (1 - a_o2 ) * w7 )  * a_h1 * (1- a_h1) * i1</t>
   </si>
+  <si>
+    <t>Output Layer</t>
+  </si>
+  <si>
+    <t>Hidden Layer</t>
+  </si>
+  <si>
+    <t>Input Layer</t>
+  </si>
+  <si>
+    <t>i1, i2 = inputs</t>
+  </si>
+  <si>
+    <t>Equations for Basic parameters</t>
+  </si>
+  <si>
+    <t>δE1/δa_o1 = δ(½ * ( t1 - a_o1)²) /δa_o1= (t1 - a_o1) * (-1) = a_o1 - t1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>δE_total/δw1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = δ(E_total)/δa_o1 * δa_o1/δo1 * δo1/δa_h1 * δa_h1/δh1 * δh1/δw1</t>
+    </r>
+  </si>
+  <si>
+    <t>η=0.1</t>
+  </si>
+  <si>
+    <t>η=0.2</t>
+  </si>
+  <si>
+    <t>η=0.5</t>
+  </si>
+  <si>
+    <t>η=0.8</t>
+  </si>
+  <si>
+    <t>η=1</t>
+  </si>
+  <si>
+    <t>η=2</t>
+  </si>
 </sst>
 </file>
 
@@ -580,7 +627,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -611,6 +658,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -624,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -646,6 +705,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -680,7 +745,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -874,11 +938,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1344740016"/>
-        <c:axId val="1344735120"/>
+        <c:axId val="934002288"/>
+        <c:axId val="933989776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1344740016"/>
+        <c:axId val="934002288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,7 +984,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1344735120"/>
+        <c:crossAx val="933989776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -928,7 +992,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1344735120"/>
+        <c:axId val="933989776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -979,7 +1043,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1344740016"/>
+        <c:crossAx val="934002288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -991,6 +1055,1291 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>E_Total for</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> different leraning rate (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>η</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Learning rate Plot'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>η=0.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Learning rate Plot'!$A$2:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0.24251985734837728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24110903876812873</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23970403156867259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23830487995320579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23691162730651111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23552431617466935</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23414298824548435</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.23276768432963732</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23139844434258416</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.23003530728721144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.22867831123726023</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22732749332153174</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22598288970888195</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.22464453559401529</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.22331246518408293</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.22198671168609313</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.22066730729513706</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.21935428318343375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.21804766949019649</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.21674749531232129</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.21545378869589749</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.214166576628539</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.21288588503253308</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.21161173875880418</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.21034416158168673</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.20908317619450248</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.20782880420593419</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.20658106613718943</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.2053399814199442</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.20410556839505828</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.20287784431205044</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.20165682532932294</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.20044252651512373</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Learning rate Plot'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>η=0.2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Learning rate Plot'!$B$2:$B$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0.24251985734837728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23970114342898322</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23690583912562505</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2341342902068855</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23138682882215905</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.22866377289884651</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22596542558768243</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.22329207475776353</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.22064399254252082</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.21802143493755069</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.21542464145089724</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.21285383480606401</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2103092206977262</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.20779098759982209</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.2052993066254179</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.20283433143747986</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.20039619820943533</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.19798502563417694</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.19560091497995413</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.19324395019140397</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.19091419803380841</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.18861170827851184</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.18633651392731257</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.18408863147353058</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.18186806119737448</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.17967478749316157</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.17750877922590497</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.17536999011475216</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.17325835914075249</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.1711738109764416</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.16911625643474981</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.16708559293478628</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.16508170498209707</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Learning rate Plot'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>η=0.5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Learning rate Plot'!$C$2:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0.24251985734837728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23549537787349017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22862020600870744</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.22189935290057158</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21533724355706674</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20893767274108918</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.202703773668297</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.19663799959953079</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1907421179707893</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18501721631430007</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1794637189063516</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.17408141283901166</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.16886948205556535</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1638265478102261</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.15895071400404875</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.1542396159006717</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.14969047082553455</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.14530012958791491</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.1410651275242675</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.13698173423274129</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.13304600124279031</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.12925380703270212</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.12560089896573273</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.12208293185828389</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.11869550301870918</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.11543418370179451</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.11229454701173039</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.10927219235630757</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.10636276660852687</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.10356198217058328</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.1008656321612144</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.8269602962661323E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9.5769884369911337E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Learning rate Plot'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>η=0.8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Learning rate Plot'!$D$2:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0.24251985734837728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23131728642977417</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22050429437507871</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.21009967584614114</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.20011810727964277</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.19056984884051159</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.18146066004951675</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.17279191160023272</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16456086243211812</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.15676106311135191</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.14938284387826717</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.14241384750356204</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.13583957209470698</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.12964389584905217</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.12380956324187031</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.11831861932755905</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.11315278510804333</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.10829377197312121</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.10372353697020928</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.9424483204908459E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9.5379611189992164E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.1572627665928302E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.7988018525968686E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.4611092183809494E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.1427999177807187E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.842573313212739E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7.5592117477869716E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.2915781633847751E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7.0386129692918964E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.7993304074767918E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.5728146097571216E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.3582154989145684E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.1547446498459911E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Learning rate Plot'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>η=1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Learning rate Plot'!$E$2:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0.24251985734837728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22854776527878509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2151917513010938</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20248615151693786</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1904549082377793</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17911099514392959</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16845661989366126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15848407315701624</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14917704036336582</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.14051217886912468</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.13246078088644664</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.12499037939225566</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.11806619845238855</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.11165239177027833</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.10571304830180256</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.10021296930959503</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.5118237483910822E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.0396607278370303E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.6017748415939219E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.1953373559056492E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.8177278008739776E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.4665315176863534E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.1395327245311377E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.8347046350994312E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.5501978053987955E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.2843275843365728E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.0355613006611825E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.8025056280016044E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5.5838944234455193E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.3785772254578659E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.1855085165816155E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.0037377988297521E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.8324004895857309E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Learning rate Plot'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>η=2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Learning rate Plot'!$F$2:$F$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0.24251985734837728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21490159884256635</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18987932614400227</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16762535191281996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14813949508015645</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13127531967647857</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.11678987307369015</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10439494052893267</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.3796722981055E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.4720552415379E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.6922979976319306E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0195330732966341E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.4362398142722599E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.9278852389163084E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.482491027939574E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0902083513451699E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.7429372470245534E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.4340023833243224E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1578846221857452E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.9100024391086813E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6865355889397926E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.4842835087706754E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.3005517883895677E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.1330610940849574E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.9798739612585584E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.839335778028651E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.7100270395771342E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.5907245673564741E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.4803698768155375E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.3780432633831283E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.282942479195206E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.1943651098189226E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.1116939452806287E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="934001744"/>
+        <c:axId val="933993040"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="934001744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>#iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="933993040"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="933993040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="934001744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1068,7 +2417,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3708,15 +5600,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>158751</xdr:rowOff>
+      <xdr:rowOff>119063</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>500063</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>97014</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3725,8 +5617,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1881188" y="1984376"/>
-          <a:ext cx="7175500" cy="2309812"/>
+          <a:off x="2119313" y="1944688"/>
+          <a:ext cx="7707312" cy="2898951"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3755,19 +5647,234 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>204107</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>156936</xdr:rowOff>
+      <xdr:colOff>283482</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>164873</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>178707</xdr:rowOff>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>4082</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="26" name="Chart 25"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>531813</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>423334</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>183443</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="531813" y="2734910"/>
+          <a:ext cx="1711854" cy="750533"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>525462</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>357186</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>174626</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="Rectangle 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="525462" y="3502026"/>
+          <a:ext cx="1665287" cy="688975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>531812</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>150811</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="Rectangle 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="531812" y="4214813"/>
+          <a:ext cx="1452562" cy="547687"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>241299</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4074,7 +6181,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4085,6 +6194,9 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="Q1" s="4" t="s">
@@ -4092,21 +6204,29 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="Q2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="J4" s="1" t="s">
-        <v>38</v>
+      <c r="K4" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="N6" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
@@ -4116,23 +6236,23 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="P8" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="N10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="O11" s="1" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
@@ -4140,282 +6260,285 @@
         <v>0.1</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="O13" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="N14" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="E15" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="N15" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T21" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="T21" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="U23" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.35">
       <c r="N27" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.35">
       <c r="O28" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="U28" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.35">
       <c r="N29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="T29" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.35">
       <c r="N30" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.35">
       <c r="N31" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.35">
       <c r="E32" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.35">
       <c r="E33" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F33" s="8">
         <v>0.5</v>
-      </c>
-      <c r="J33" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="F34" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="G34" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="J34" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="K34" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="M34" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="M34" s="5" t="s">
+      <c r="N34" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="N34" s="5" t="s">
+      <c r="O34" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O34" s="5" t="s">
+      <c r="P34" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P34" s="5" t="s">
+      <c r="Q34" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="Q34" s="5" t="s">
+      <c r="R34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="R34" s="5" t="s">
+      <c r="S34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S34" s="5" t="s">
+      <c r="T34" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="T34" s="5" t="s">
+      <c r="U34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="U34" s="5" t="s">
+      <c r="V34" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="V34" s="5" t="s">
+      <c r="W34" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="W34" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="X34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z34" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB34" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="Y34" s="5" t="s">
+      <c r="AC34" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="Z34" s="5" t="s">
+      <c r="AD34" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AA34" s="5" t="s">
+      <c r="AE34" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="AB34" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC34" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD34" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE34" s="5" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4471,19 +6594,19 @@
       <c r="P35" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="Q35" s="2">
+      <c r="Q35" s="11">
         <f>M35*J35+N35*L35</f>
         <v>0.43253035715804738</v>
       </c>
-      <c r="R35" s="2">
+      <c r="R35" s="11">
         <f>1/(1+EXP(-Q35))</f>
         <v>0.60647773220672796</v>
       </c>
-      <c r="S35" s="2">
+      <c r="S35" s="11">
         <f>O35*J35+P35*L35</f>
         <v>0.53428015393499717</v>
       </c>
-      <c r="T35" s="2">
+      <c r="T35" s="11">
         <f>1/(1+EXP(-S35))</f>
         <v>0.63048083545063482</v>
       </c>
@@ -4495,7 +6618,7 @@
         <f>0.5*(T35-B35)^2</f>
         <v>6.4627014839136757E-2</v>
       </c>
-      <c r="W35" s="2">
+      <c r="W35" s="12">
         <f>U35+V35</f>
         <v>0.24251985734837728</v>
       </c>
@@ -4593,19 +6716,19 @@
         <f t="shared" si="1"/>
         <v>0.57138462414003188</v>
       </c>
-      <c r="Q36" s="2">
+      <c r="Q36" s="11">
         <f>M36*J36+N36*L36</f>
         <v>0.39567922152806312</v>
       </c>
-      <c r="R36" s="2">
+      <c r="R36" s="11">
         <f>1/(1+EXP(-Q36))</f>
         <v>0.59764910542281569</v>
       </c>
-      <c r="S36" s="2">
+      <c r="S36" s="11">
         <f>O36*J36+P36*L36</f>
         <v>0.55595230848741006</v>
       </c>
-      <c r="T36" s="2">
+      <c r="T36" s="11">
         <f>1/(1+EXP(-S36))</f>
         <v>0.63551546628555877</v>
       </c>
@@ -4617,7 +6740,7 @@
         <f>0.5*(T36-B36)^2</f>
         <v>6.2829642321372406E-2</v>
       </c>
-      <c r="W36" s="2">
+      <c r="W36" s="12">
         <f>U36+V36</f>
         <v>0.23549537787349017</v>
       </c>
@@ -4715,19 +6838,19 @@
         <f t="shared" ref="P37:P67" si="13">P36-$F$33*AE36</f>
         <v>0.59234829178874815</v>
       </c>
-      <c r="Q37" s="2">
+      <c r="Q37" s="11">
         <f t="shared" ref="Q37:Q67" si="14">M37*J37+N37*L37</f>
         <v>0.35910251323992115</v>
       </c>
-      <c r="R37" s="2">
+      <c r="R37" s="11">
         <f t="shared" ref="R37:R67" si="15">1/(1+EXP(-Q37))</f>
         <v>0.58882316047387184</v>
       </c>
-      <c r="S37" s="2">
+      <c r="S37" s="11">
         <f t="shared" ref="S37:S67" si="16">O37*J37+P37*L37</f>
         <v>0.57720004570236483</v>
       </c>
-      <c r="T37" s="2">
+      <c r="T37" s="11">
         <f t="shared" ref="T37:T67" si="17">1/(1+EXP(-S37))</f>
         <v>0.64042288273336123</v>
       </c>
@@ -4739,7 +6862,7 @@
         <f t="shared" ref="V37:V67" si="19">0.5*(T37-B37)^2</f>
         <v>6.1102080458226654E-2</v>
       </c>
-      <c r="W37" s="2">
+      <c r="W37" s="12">
         <f t="shared" ref="W37:W67" si="20">U37+V37</f>
         <v>0.22862020600870744</v>
       </c>
@@ -4837,19 +6960,19 @@
         <f t="shared" si="13"/>
         <v>0.61290070394283069</v>
       </c>
-      <c r="Q38" s="2">
+      <c r="Q38" s="11">
         <f t="shared" si="14"/>
         <v>0.32283095172279641</v>
       </c>
-      <c r="R38" s="2">
+      <c r="R38" s="11">
         <f t="shared" si="15"/>
         <v>0.58001402141982483</v>
       </c>
-      <c r="S38" s="2">
+      <c r="S38" s="11">
         <f t="shared" si="16"/>
         <v>0.59803345448386924</v>
       </c>
-      <c r="T38" s="2">
+      <c r="T38" s="11">
         <f t="shared" si="17"/>
         <v>0.64520626283828375</v>
       </c>
@@ -4861,7 +6984,7 @@
         <f t="shared" si="19"/>
         <v>5.944136059297133E-2</v>
       </c>
-      <c r="W38" s="2">
+      <c r="W38" s="12">
         <f t="shared" si="20"/>
         <v>0.22189935290057158</v>
       </c>
@@ -4959,19 +7082,19 @@
         <f t="shared" si="13"/>
         <v>0.63305153995904673</v>
       </c>
-      <c r="Q39" s="2">
+      <c r="Q39" s="11">
         <f t="shared" si="14"/>
         <v>0.2868936336471819</v>
       </c>
-      <c r="R39" s="2">
+      <c r="R39" s="11">
         <f t="shared" si="15"/>
         <v>0.5712354735096804</v>
       </c>
-      <c r="S39" s="2">
+      <c r="S39" s="11">
         <f t="shared" si="16"/>
         <v>0.61846257322780285</v>
       </c>
-      <c r="T39" s="2">
+      <c r="T39" s="11">
         <f t="shared" si="17"/>
         <v>0.64986880415272352</v>
       </c>
@@ -4983,7 +7106,7 @@
         <f t="shared" si="19"/>
         <v>5.7844615194249167E-2</v>
       </c>
-      <c r="W39" s="2">
+      <c r="W39" s="12">
         <f t="shared" si="20"/>
         <v>0.21533724355706674</v>
       </c>
@@ -5081,19 +7204,19 @@
         <f t="shared" si="13"/>
         <v>0.65281042559392544</v>
       </c>
-      <c r="Q40" s="2">
+      <c r="Q40" s="11">
         <f t="shared" si="14"/>
         <v>0.25131786909749387</v>
       </c>
-      <c r="R40" s="2">
+      <c r="R40" s="11">
         <f t="shared" si="15"/>
         <v>0.56250084676327505</v>
       </c>
-      <c r="S40" s="2">
+      <c r="S40" s="11">
         <f t="shared" si="16"/>
         <v>0.63849735787940443</v>
       </c>
-      <c r="T40" s="2">
+      <c r="T40" s="11">
         <f t="shared" si="17"/>
         <v>0.65441370735972781</v>
       </c>
@@ -5105,7 +7228,7 @@
         <f t="shared" si="19"/>
         <v>5.6309079904021196E-2</v>
       </c>
-      <c r="W40" s="2">
+      <c r="W40" s="12">
         <f t="shared" si="20"/>
         <v>0.20893767274108918</v>
       </c>
@@ -5203,19 +7326,19 @@
         <f t="shared" si="13"/>
         <v>0.67218690532452696</v>
       </c>
-      <c r="Q41" s="2">
+      <c r="Q41" s="11">
         <f t="shared" si="14"/>
         <v>0.21612904596375726</v>
       </c>
-      <c r="R41" s="2">
+      <c r="R41" s="11">
         <f t="shared" si="15"/>
         <v>0.55382291082758639</v>
       </c>
-      <c r="S41" s="2">
+      <c r="S41" s="11">
         <f t="shared" si="16"/>
         <v>0.65814765454416513</v>
       </c>
-      <c r="T41" s="2">
+      <c r="T41" s="11">
         <f t="shared" si="17"/>
         <v>0.65884416206926832</v>
       </c>
@@ -5227,7 +7350,7 @@
         <f t="shared" si="19"/>
         <v>5.4832094497802512E-2</v>
       </c>
-      <c r="W41" s="2">
+      <c r="W41" s="12">
         <f t="shared" si="20"/>
         <v>0.202703773668297</v>
       </c>
@@ -5325,19 +7448,19 @@
         <f t="shared" si="13"/>
         <v>0.69119041856821661</v>
       </c>
-      <c r="Q42" s="2">
+      <c r="Q42" s="11">
         <f t="shared" si="14"/>
         <v>0.18135052372830501</v>
       </c>
-      <c r="R42" s="2">
+      <c r="R42" s="11">
         <f t="shared" si="15"/>
         <v>0.54521378284696775</v>
       </c>
-      <c r="S42" s="2">
+      <c r="S42" s="11">
         <f t="shared" si="16"/>
         <v>0.67742317625119652</v>
       </c>
-      <c r="T42" s="2">
+      <c r="T42" s="11">
         <f t="shared" si="17"/>
         <v>0.66316333460013943</v>
       </c>
@@ -5349,7 +7472,7 @@
         <f t="shared" si="19"/>
         <v>5.3411102924850205E-2</v>
       </c>
-      <c r="W42" s="2">
+      <c r="W42" s="12">
         <f t="shared" si="20"/>
         <v>0.19663799959953079</v>
       </c>
@@ -5447,19 +7570,19 @@
         <f t="shared" si="13"/>
         <v>0.70983027943521371</v>
       </c>
-      <c r="Q43" s="2">
+      <c r="Q43" s="11">
         <f t="shared" si="14"/>
         <v>0.14700355697961393</v>
       </c>
-      <c r="R43" s="2">
+      <c r="R43" s="11">
         <f t="shared" si="15"/>
         <v>0.53668484958669704</v>
       </c>
-      <c r="S43" s="2">
+      <c r="S43" s="11">
         <f t="shared" si="16"/>
         <v>0.69633348347922008</v>
       </c>
-      <c r="T43" s="2">
+      <c r="T43" s="11">
         <f t="shared" si="17"/>
         <v>0.66737435756372843</v>
       </c>
@@ -5471,7 +7594,7 @@
         <f t="shared" si="19"/>
         <v>5.2043652578708473E-2</v>
       </c>
-      <c r="W43" s="2">
+      <c r="W43" s="12">
         <f t="shared" si="20"/>
         <v>0.1907421179707893</v>
       </c>
@@ -5569,19 +7692,19 @@
         <f t="shared" si="13"/>
         <v>0.72811565966656466</v>
       </c>
-      <c r="Q44" s="2">
+      <c r="Q44" s="11">
         <f t="shared" si="14"/>
         <v>0.11310724819072746</v>
       </c>
-      <c r="R44" s="2">
+      <c r="R44" s="11">
         <f t="shared" si="15"/>
         <v>0.528246704538198</v>
       </c>
-      <c r="S44" s="2">
+      <c r="S44" s="11">
         <f t="shared" si="16"/>
         <v>0.71488796807047206</v>
       </c>
-      <c r="T44" s="2">
+      <c r="T44" s="11">
         <f t="shared" si="17"/>
         <v>0.67148032107278233</v>
       </c>
@@ -5593,7 +7716,7 @@
         <f t="shared" si="19"/>
         <v>5.0727392931948917E-2</v>
       </c>
-      <c r="W44" s="2">
+      <c r="W44" s="12">
         <f t="shared" si="20"/>
         <v>0.18501721631430007</v>
       </c>
@@ -5691,19 +7814,19 @@
         <f t="shared" si="13"/>
         <v>0.74605557443107273</v>
       </c>
-      <c r="Q45" s="2">
+      <c r="Q45" s="11">
         <f t="shared" si="14"/>
         <v>7.9678528585628225E-2</v>
       </c>
-      <c r="R45" s="2">
+      <c r="R45" s="11">
         <f t="shared" si="15"/>
         <v>0.51990910023858694</v>
       </c>
-      <c r="S45" s="2">
+      <c r="S45" s="11">
         <f t="shared" si="16"/>
         <v>0.73309584017609197</v>
       </c>
-      <c r="T45" s="2">
+      <c r="T45" s="11">
         <f t="shared" si="17"/>
         <v>0.67548426540699447</v>
       </c>
@@ -5715,7 +7838,7 @@
         <f t="shared" si="19"/>
         <v>4.9460073653288944E-2</v>
       </c>
-      <c r="W45" s="2">
+      <c r="W45" s="12">
         <f t="shared" si="20"/>
         <v>0.1794637189063516</v>
       </c>
@@ -5813,19 +7936,19 @@
         <f t="shared" si="13"/>
         <v>0.76365887067675997</v>
       </c>
-      <c r="Q46" s="2">
+      <c r="Q46" s="11">
         <f t="shared" si="14"/>
         <v>4.6732165307280533E-2</v>
       </c>
-      <c r="R46" s="2">
+      <c r="R46" s="11">
         <f t="shared" si="15"/>
         <v>0.51168091557949791</v>
       </c>
-      <c r="S46" s="2">
+      <c r="S46" s="11">
         <f t="shared" si="16"/>
         <v>0.75096611789717205</v>
       </c>
-      <c r="T46" s="2">
+      <c r="T46" s="11">
         <f t="shared" si="17"/>
         <v>0.67938917497720719</v>
       </c>
@@ -5837,7 +7960,7 @@
         <f t="shared" si="19"/>
         <v>4.8239542310670007E-2</v>
       </c>
-      <c r="W46" s="2">
+      <c r="W46" s="12">
         <f t="shared" si="20"/>
         <v>0.17408141283901166</v>
       </c>
@@ -5935,19 +8058,19 @@
         <f t="shared" si="13"/>
         <v>0.78093421775496885</v>
       </c>
-      <c r="Q47" s="2">
+      <c r="Q47" s="11">
         <f t="shared" si="14"/>
         <v>1.4280792611373702E-2</v>
       </c>
-      <c r="R47" s="2">
+      <c r="R47" s="11">
         <f t="shared" si="15"/>
         <v>0.50357013747825452</v>
       </c>
-      <c r="S47" s="2">
+      <c r="S47" s="11">
         <f t="shared" si="16"/>
         <v>0.76850761930783684</v>
       </c>
-      <c r="T47" s="2">
+      <c r="T47" s="11">
         <f t="shared" si="17"/>
         <v>0.68319797344080724</v>
       </c>
@@ -5959,7 +8082,7 @@
         <f t="shared" si="19"/>
         <v>4.7063741750413807E-2</v>
       </c>
-      <c r="W47" s="2">
+      <c r="W47" s="12">
         <f t="shared" si="20"/>
         <v>0.16886948205556535</v>
       </c>
@@ -6057,19 +8180,19 @@
         <f t="shared" si="13"/>
         <v>0.7978901000576879</v>
       </c>
-      <c r="Q48" s="2">
+      <c r="Q48" s="11">
         <f t="shared" si="14"/>
         <v>-1.7665035552750206E-2</v>
       </c>
-      <c r="R48" s="2">
+      <c r="R48" s="11">
         <f t="shared" si="15"/>
         <v>0.49558385595064219</v>
       </c>
-      <c r="S48" s="2">
+      <c r="S48" s="11">
         <f t="shared" si="16"/>
         <v>0.7857289565698895</v>
       </c>
-      <c r="T48" s="2">
+      <c r="T48" s="11">
         <f t="shared" si="17"/>
         <v>0.68691351983211424</v>
       </c>
@@ -6081,7 +8204,7 @@
         <f t="shared" si="19"/>
         <v>4.5930707230279103E-2</v>
       </c>
-      <c r="W48" s="2">
+      <c r="W48" s="12">
         <f t="shared" si="20"/>
         <v>0.1638265478102261</v>
       </c>
@@ -6179,19 +8302,19 @@
         <f t="shared" si="13"/>
         <v>0.8145348114307035</v>
       </c>
-      <c r="Q49" s="2">
+      <c r="Q49" s="11">
         <f t="shared" si="14"/>
         <v>-4.9096774448368824E-2</v>
       </c>
-      <c r="R49" s="2">
+      <c r="R49" s="11">
         <f t="shared" si="15"/>
         <v>0.48772827136547742</v>
       </c>
-      <c r="S49" s="2">
+      <c r="S49" s="11">
         <f t="shared" si="16"/>
         <v>0.80263853187211409</v>
       </c>
-      <c r="T49" s="2">
+      <c r="T49" s="11">
         <f t="shared" si="17"/>
         <v>0.69053860558287272</v>
       </c>
@@ -6203,7 +8326,7 @@
         <f t="shared" si="19"/>
         <v>4.4838563373125133E-2</v>
       </c>
-      <c r="W49" s="2">
+      <c r="W49" s="12">
         <f t="shared" si="20"/>
         <v>0.15895071400404875</v>
       </c>
@@ -6301,19 +8424,19 @@
         <f t="shared" si="13"/>
         <v>0.83087645114642006</v>
       </c>
-      <c r="Q50" s="2">
+      <c r="Q50" s="11">
         <f t="shared" si="14"/>
         <v>-8.0007801935383566E-2</v>
       </c>
-      <c r="R50" s="2">
+      <c r="R50" s="11">
         <f t="shared" si="15"/>
         <v>0.48000871247832433</v>
       </c>
-      <c r="S50" s="2">
+      <c r="S50" s="11">
         <f t="shared" si="16"/>
         <v>0.81924453495081551</v>
       </c>
-      <c r="T50" s="2">
+      <c r="T50" s="11">
         <f t="shared" si="17"/>
         <v>0.6940759523191613</v>
       </c>
@@ -6325,7 +8448,7 @@
         <f t="shared" si="19"/>
         <v>4.3785520997905641E-2</v>
       </c>
-      <c r="W50" s="2">
+      <c r="W50" s="12">
         <f t="shared" si="20"/>
         <v>0.1542396159006717</v>
       </c>
@@ -6423,19 +8546,19 @@
         <f t="shared" si="13"/>
         <v>0.84692292124043145</v>
       </c>
-      <c r="Q51" s="2">
+      <c r="Q51" s="11">
         <f t="shared" si="14"/>
         <v>-0.11039331933101179</v>
       </c>
-      <c r="R51" s="2">
+      <c r="R51" s="11">
         <f t="shared" si="15"/>
         <v>0.47242966373210787</v>
       </c>
-      <c r="S51" s="2">
+      <c r="S51" s="11">
         <f t="shared" si="16"/>
         <v>0.83555494197116553</v>
       </c>
-      <c r="T51" s="2">
+      <c r="T51" s="11">
         <f t="shared" si="17"/>
         <v>0.69752821033187018</v>
       </c>
@@ -6447,7 +8570,7 @@
         <f t="shared" si="19"/>
         <v>4.276987387583938E-2</v>
       </c>
-      <c r="W51" s="2">
+      <c r="W51" s="12">
         <f t="shared" si="20"/>
         <v>0.14969047082553455</v>
       </c>
@@ -6545,19 +8668,19 @@
         <f t="shared" si="13"/>
         <v>0.86268192503502306</v>
       </c>
-      <c r="Q52" s="2">
+      <c r="Q52" s="11">
         <f t="shared" si="14"/>
         <v>-0.14025024266229383</v>
       </c>
-      <c r="R52" s="2">
+      <c r="R52" s="11">
         <f t="shared" si="15"/>
         <v>0.46499480026955137</v>
       </c>
-      <c r="S52" s="2">
+      <c r="S52" s="11">
         <f t="shared" si="16"/>
         <v>0.85157751557112227</v>
       </c>
-      <c r="T52" s="2">
+      <c r="T52" s="11">
         <f t="shared" si="17"/>
         <v>0.70089795762827811</v>
       </c>
@@ -6569,7 +8692,7 @@
         <f t="shared" si="19"/>
         <v>4.1789995451750439E-2</v>
       </c>
-      <c r="W52" s="2">
+      <c r="W52" s="12">
         <f t="shared" si="20"/>
         <v>0.14530012958791491</v>
       </c>
@@ -6667,19 +8790,19 @@
         <f t="shared" si="13"/>
         <v>0.87816096669063171</v>
       </c>
-      <c r="Q53" s="2">
+      <c r="Q53" s="11">
         <f t="shared" si="14"/>
         <v>-0.16957708706685529</v>
       </c>
-      <c r="R53" s="2">
+      <c r="R53" s="11">
         <f t="shared" si="15"/>
         <v>0.45770702911744121</v>
       </c>
-      <c r="S53" s="2">
+      <c r="S53" s="11">
         <f t="shared" si="16"/>
         <v>0.86731980589079716</v>
       </c>
-      <c r="T53" s="2">
+      <c r="T53" s="11">
         <f t="shared" si="17"/>
         <v>0.7041876994820383</v>
       </c>
@@ -6691,7 +8814,7 @@
         <f t="shared" si="19"/>
         <v>4.0844335563684823E-2</v>
       </c>
-      <c r="W53" s="2">
+      <c r="W53" s="12">
         <f t="shared" si="20"/>
         <v>0.1410651275242675</v>
       </c>
@@ -6789,19 +8912,19 @@
         <f t="shared" si="13"/>
         <v>0.89336735164285597</v>
       </c>
-      <c r="Q54" s="2">
+      <c r="Q54" s="11">
         <f t="shared" si="14"/>
         <v>-0.19837384688278842</v>
       </c>
-      <c r="R54" s="2">
+      <c r="R54" s="11">
         <f t="shared" si="15"/>
         <v>0.45056853506539729</v>
       </c>
-      <c r="S54" s="2">
+      <c r="S54" s="11">
         <f t="shared" si="16"/>
         <v>0.88278915242999156</v>
       </c>
-      <c r="T54" s="2">
+      <c r="T54" s="11">
         <f t="shared" si="17"/>
         <v>0.70739986840800584</v>
       </c>
@@ -6813,7 +8936,7 @@
         <f t="shared" si="19"/>
         <v>3.9931417187906208E-2</v>
       </c>
-      <c r="W54" s="2">
+      <c r="W54" s="12">
         <f t="shared" si="20"/>
         <v>0.13698173423274129</v>
       </c>
@@ -6911,19 +9034,19 @@
         <f t="shared" si="13"/>
         <v>0.90830818779787592</v>
       </c>
-      <c r="Q55" s="2">
+      <c r="Q55" s="11">
         <f t="shared" si="14"/>
         <v>-0.22664187371343389</v>
       </c>
-      <c r="R55" s="2">
+      <c r="R55" s="11">
         <f t="shared" si="15"/>
         <v>0.44358082986132441</v>
       </c>
-      <c r="S55" s="2">
+      <c r="S55" s="11">
         <f t="shared" si="16"/>
         <v>0.89799268659509257</v>
       </c>
-      <c r="T55" s="2">
+      <c r="T55" s="11">
         <f t="shared" si="17"/>
         <v>0.7105368244967758</v>
       </c>
@@ -6935,7 +9058,7 @@
         <f t="shared" si="19"/>
         <v>3.9049833231172941E-2</v>
       </c>
-      <c r="W55" s="2">
+      <c r="W55" s="12">
         <f t="shared" si="20"/>
         <v>0.13304600124279031</v>
       </c>
@@ -7033,19 +9156,19 @@
         <f t="shared" si="13"/>
         <v>0.92299038737313188</v>
       </c>
-      <c r="Q56" s="2">
+      <c r="Q56" s="11">
         <f t="shared" si="14"/>
         <v>-0.25438375447421907</v>
       </c>
-      <c r="R56" s="2">
+      <c r="R56" s="11">
         <f t="shared" si="15"/>
         <v>0.43674480347152189</v>
       </c>
-      <c r="S56" s="2">
+      <c r="S56" s="11">
         <f t="shared" si="16"/>
         <v>0.91293733481349304</v>
       </c>
-      <c r="T56" s="2">
+      <c r="T56" s="11">
         <f t="shared" si="17"/>
         <v>0.71360085605151302</v>
       </c>
@@ -7057,7 +9180,7 @@
         <f t="shared" si="19"/>
         <v>3.819824338772821E-2</v>
       </c>
-      <c r="W56" s="2">
+      <c r="W56" s="12">
         <f t="shared" si="20"/>
         <v>0.12925380703270212</v>
       </c>
@@ -7155,19 +9278,19 @@
         <f t="shared" si="13"/>
         <v>0.93742066928286838</v>
       </c>
-      <c r="Q57" s="2">
+      <c r="Q57" s="11">
         <f t="shared" si="14"/>
         <v>-0.2816031911404927</v>
       </c>
-      <c r="R57" s="2">
+      <c r="R57" s="11">
         <f t="shared" si="15"/>
         <v>0.43006077629582051</v>
       </c>
-      <c r="S57" s="2">
+      <c r="S57" s="11">
         <f t="shared" si="16"/>
         <v>0.92762982210920542</v>
       </c>
-      <c r="T57" s="2">
+      <c r="T57" s="11">
         <f t="shared" si="17"/>
         <v>0.71659418047668022</v>
       </c>
@@ -7179,7 +9302,7 @@
         <f t="shared" si="19"/>
         <v>3.7375371074609053E-2</v>
       </c>
-      <c r="W57" s="2">
+      <c r="W57" s="12">
         <f t="shared" si="20"/>
         <v>0.12560089896573273</v>
       </c>
@@ -7277,19 +9400,19 @@
         <f t="shared" si="13"/>
         <v>0.95160556197972634</v>
       </c>
-      <c r="Q58" s="2">
+      <c r="Q58" s="11">
         <f t="shared" si="14"/>
         <v>-0.30830488362910835</v>
       </c>
-      <c r="R58" s="2">
+      <c r="R58" s="11">
         <f t="shared" si="15"/>
         <v>0.42352855137861528</v>
       </c>
-      <c r="S58" s="2">
+      <c r="S58" s="11">
         <f t="shared" si="16"/>
         <v>0.94207667604733758</v>
       </c>
-      <c r="T58" s="2">
+      <c r="T58" s="11">
         <f t="shared" si="17"/>
         <v>0.71951894537459427</v>
       </c>
@@ -7301,7 +9424,7 @@
         <f t="shared" si="19"/>
         <v>3.6580000455635857E-2</v>
       </c>
-      <c r="W58" s="2">
+      <c r="W58" s="12">
         <f t="shared" si="20"/>
         <v>0.12208293185828389</v>
       </c>
@@ -7399,19 +9522,19 @@
         <f t="shared" si="13"/>
         <v>0.96555140667403083</v>
       </c>
-      <c r="Q59" s="2">
+      <c r="Q59" s="11">
         <f t="shared" si="14"/>
         <v>-0.33449441697156224</v>
       </c>
-      <c r="R59" s="2">
+      <c r="R59" s="11">
         <f t="shared" si="15"/>
         <v>0.41714746580816897</v>
       </c>
-      <c r="S59" s="2">
+      <c r="S59" s="11">
         <f t="shared" si="16"/>
         <v>0.95628423096768289</v>
       </c>
-      <c r="T59" s="2">
+      <c r="T59" s="11">
         <f t="shared" si="17"/>
         <v>0.72237722981142982</v>
       </c>
@@ -7423,7 +9546,7 @@
         <f t="shared" si="19"/>
         <v>3.5810973561702118E-2</v>
       </c>
-      <c r="W59" s="2">
+      <c r="W59" s="12">
         <f t="shared" si="20"/>
         <v>0.11869550301870918</v>
       </c>
@@ -7521,19 +9644,19 @@
         <f t="shared" si="13"/>
         <v>0.97926436086184931</v>
       </c>
-      <c r="Q60" s="2">
+      <c r="Q60" s="11">
         <f t="shared" si="14"/>
         <v>-0.36017815367961292</v>
       </c>
-      <c r="R60" s="2">
+      <c r="R60" s="11">
         <f t="shared" si="15"/>
         <v>0.41091644064344346</v>
       </c>
-      <c r="S60" s="2">
+      <c r="S60" s="11">
         <f t="shared" si="16"/>
         <v>0.9702586324388599</v>
       </c>
-      <c r="T60" s="2">
+      <c r="T60" s="11">
         <f t="shared" si="17"/>
         <v>0.72517104571935243</v>
       </c>
@@ -7545,7 +9668,7 @@
         <f t="shared" si="19"/>
         <v>3.506718751269066E-2</v>
       </c>
-      <c r="W60" s="2">
+      <c r="W60" s="12">
         <f t="shared" si="20"/>
         <v>0.11543418370179451</v>
       </c>
@@ -7643,19 +9766,19 @@
         <f t="shared" si="13"/>
         <v>0.99275040210135412</v>
       </c>
-      <c r="Q61" s="2">
+      <c r="Q61" s="11">
         <f t="shared" si="14"/>
         <v>-0.38536313197020666</v>
       </c>
-      <c r="R61" s="2">
+      <c r="R61" s="11">
         <f t="shared" si="15"/>
         <v>0.40483402884578767</v>
       </c>
-      <c r="S61" s="2">
+      <c r="S61" s="11">
         <f t="shared" si="16"/>
         <v>0.9840058418743679</v>
       </c>
-      <c r="T61" s="2">
+      <c r="T61" s="11">
         <f t="shared" si="17"/>
         <v>0.72790233940596782</v>
       </c>
@@ -7667,7 +9790,7 @@
         <f t="shared" si="19"/>
         <v>3.4347591844432243E-2</v>
       </c>
-      <c r="W61" s="2">
+      <c r="W61" s="12">
         <f t="shared" si="20"/>
         <v>0.11229454701173039</v>
       </c>
@@ -7765,19 +9888,19 @@
         <f t="shared" si="13"/>
         <v>1.0060153319846006</v>
       </c>
-      <c r="Q62" s="2">
+      <c r="Q62" s="11">
         <f t="shared" si="14"/>
         <v>-0.4100569703079785</v>
       </c>
-      <c r="R62" s="2">
+      <c r="R62" s="11">
         <f t="shared" si="15"/>
         <v>0.39889846081917091</v>
       </c>
-      <c r="S62" s="2">
+      <c r="S62" s="11">
         <f t="shared" si="16"/>
         <v>0.99753164126063465</v>
       </c>
-      <c r="T62" s="2">
+      <c r="T62" s="11">
         <f t="shared" si="17"/>
         <v>0.73057299314625135</v>
       </c>
@@ -7789,7 +9912,7 @@
         <f t="shared" si="19"/>
         <v>3.3651185942547471E-2</v>
       </c>
-      <c r="W62" s="2">
+      <c r="W62" s="12">
         <f t="shared" si="20"/>
         <v>0.10927219235630757</v>
       </c>
@@ -7887,19 +10010,19 @@
         <f t="shared" si="13"/>
         <v>1.0190647802585933</v>
       </c>
-      <c r="Q63" s="2">
+      <c r="Q63" s="11">
         <f t="shared" si="14"/>
         <v>-0.43426777854183329</v>
       </c>
-      <c r="R63" s="2">
+      <c r="R63" s="11">
         <f t="shared" si="15"/>
         <v>0.39310768727553019</v>
       </c>
-      <c r="S63" s="2">
+      <c r="S63" s="11">
         <f t="shared" si="16"/>
         <v>1.0108416379547753</v>
       </c>
-      <c r="T63" s="2">
+      <c r="T63" s="11">
         <f t="shared" si="17"/>
         <v>0.73318482683562425</v>
       </c>
@@ -7911,7 +10034,7 @@
         <f t="shared" si="19"/>
         <v>3.297701658372415E-2</v>
       </c>
-      <c r="W63" s="2">
+      <c r="W63" s="12">
         <f t="shared" si="20"/>
         <v>0.10636276660852687</v>
       </c>
@@ -8009,19 +10132,19 @@
         <f t="shared" si="13"/>
         <v>1.0319042090555344</v>
       </c>
-      <c r="Q64" s="2">
+      <c r="Q64" s="11">
         <f t="shared" si="14"/>
         <v>-0.45800407575708391</v>
       </c>
-      <c r="R64" s="2">
+      <c r="R64" s="11">
         <f t="shared" si="15"/>
         <v>0.38745941924039184</v>
       </c>
-      <c r="S64" s="2">
+      <c r="S64" s="11">
         <f t="shared" si="16"/>
         <v>1.0239412695164327</v>
       </c>
-      <c r="T64" s="2">
+      <c r="T64" s="11">
         <f t="shared" si="17"/>
         <v>0.73573959968592695</v>
       </c>
@@ -8033,7 +10156,7 @@
         <f t="shared" si="19"/>
         <v>3.232417558393634E-2</v>
       </c>
-      <c r="W64" s="2">
+      <c r="W64" s="12">
         <f t="shared" si="20"/>
         <v>0.10356198217058328</v>
       </c>
@@ -8131,19 +10254,19 @@
         <f t="shared" si="13"/>
         <v>1.0445389171975052</v>
       </c>
-      <c r="Q65" s="2">
+      <c r="Q65" s="11">
         <f t="shared" si="14"/>
         <v>-0.48127471483533635</v>
       </c>
-      <c r="R65" s="2">
+      <c r="R65" s="11">
         <f t="shared" si="15"/>
         <v>0.3819511650981523</v>
       </c>
-      <c r="S65" s="2">
+      <c r="S65" s="11">
         <f t="shared" si="16"/>
         <v>1.0368358085438367</v>
       </c>
-      <c r="T65" s="2">
+      <c r="T65" s="11">
         <f t="shared" si="17"/>
         <v>0.73823901194872177</v>
       </c>
@@ -8155,7 +10278,7 @@
         <f t="shared" si="19"/>
         <v>3.1691797552277925E-2</v>
       </c>
-      <c r="W65" s="2">
+      <c r="W65" s="12">
         <f t="shared" si="20"/>
         <v>0.1008656321612144</v>
       </c>
@@ -8253,19 +10376,19 @@
         <f t="shared" si="13"/>
         <v>1.0569740445455729</v>
       </c>
-      <c r="Q66" s="2">
+      <c r="Q66" s="11">
         <f t="shared" si="14"/>
         <v>-0.50408881360910596</v>
       </c>
-      <c r="R66" s="2">
+      <c r="R66" s="11">
         <f t="shared" si="15"/>
         <v>0.37658026464674843</v>
       </c>
-      <c r="S66" s="2">
+      <c r="S66" s="11">
         <f t="shared" si="16"/>
         <v>1.0495303674892</v>
       </c>
-      <c r="T66" s="2">
+      <c r="T66" s="11">
         <f t="shared" si="17"/>
         <v>0.74068470665271546</v>
       </c>
@@ -8277,7 +10400,7 @@
         <f t="shared" si="19"/>
         <v>3.107905774842127E-2</v>
       </c>
-      <c r="W66" s="2">
+      <c r="W66" s="12">
         <f t="shared" si="20"/>
         <v>9.8269602962661323E-2</v>
       </c>
@@ -8375,19 +10498,19 @@
         <f t="shared" si="13"/>
         <v>1.0692145763675207</v>
       </c>
-      <c r="Q67" s="2">
+      <c r="Q67" s="11">
         <f t="shared" si="14"/>
         <v>-0.52645569241487777</v>
       </c>
-      <c r="R67" s="2">
+      <c r="R67" s="11">
         <f t="shared" si="15"/>
         <v>0.37134392018881912</v>
       </c>
-      <c r="S67" s="2">
+      <c r="S67" s="11">
         <f t="shared" si="16"/>
         <v>1.062029903432868</v>
       </c>
-      <c r="T67" s="2">
+      <c r="T67" s="11">
         <f t="shared" si="17"/>
         <v>0.74307827134413829</v>
       </c>
@@ -8399,7 +10522,7 @@
         <f t="shared" si="19"/>
         <v>3.0485170041199498E-2</v>
       </c>
-      <c r="W67" s="2">
+      <c r="W67" s="12">
         <f t="shared" si="20"/>
         <v>9.5769884369911337E-2</v>
       </c>
@@ -8441,4 +10564,700 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0.24251985734837728</v>
+      </c>
+      <c r="B2">
+        <v>0.24251985734837728</v>
+      </c>
+      <c r="C2">
+        <v>0.24251985734837728</v>
+      </c>
+      <c r="D2">
+        <v>0.24251985734837728</v>
+      </c>
+      <c r="E2">
+        <v>0.24251985734837728</v>
+      </c>
+      <c r="F2">
+        <v>0.24251985734837728</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>0.24110903876812873</v>
+      </c>
+      <c r="B3">
+        <v>0.23970114342898322</v>
+      </c>
+      <c r="C3">
+        <v>0.23549537787349017</v>
+      </c>
+      <c r="D3">
+        <v>0.23131728642977417</v>
+      </c>
+      <c r="E3">
+        <v>0.22854776527878509</v>
+      </c>
+      <c r="F3">
+        <v>0.21490159884256635</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>0.23970403156867259</v>
+      </c>
+      <c r="B4">
+        <v>0.23690583912562505</v>
+      </c>
+      <c r="C4">
+        <v>0.22862020600870744</v>
+      </c>
+      <c r="D4">
+        <v>0.22050429437507871</v>
+      </c>
+      <c r="E4">
+        <v>0.2151917513010938</v>
+      </c>
+      <c r="F4">
+        <v>0.18987932614400227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0.23830487995320579</v>
+      </c>
+      <c r="B5">
+        <v>0.2341342902068855</v>
+      </c>
+      <c r="C5">
+        <v>0.22189935290057158</v>
+      </c>
+      <c r="D5">
+        <v>0.21009967584614114</v>
+      </c>
+      <c r="E5">
+        <v>0.20248615151693786</v>
+      </c>
+      <c r="F5">
+        <v>0.16762535191281996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0.23691162730651111</v>
+      </c>
+      <c r="B6">
+        <v>0.23138682882215905</v>
+      </c>
+      <c r="C6">
+        <v>0.21533724355706674</v>
+      </c>
+      <c r="D6">
+        <v>0.20011810727964277</v>
+      </c>
+      <c r="E6">
+        <v>0.1904549082377793</v>
+      </c>
+      <c r="F6">
+        <v>0.14813949508015645</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0.23552431617466935</v>
+      </c>
+      <c r="B7">
+        <v>0.22866377289884651</v>
+      </c>
+      <c r="C7">
+        <v>0.20893767274108918</v>
+      </c>
+      <c r="D7">
+        <v>0.19056984884051159</v>
+      </c>
+      <c r="E7">
+        <v>0.17911099514392959</v>
+      </c>
+      <c r="F7">
+        <v>0.13127531967647857</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>0.23414298824548435</v>
+      </c>
+      <c r="B8">
+        <v>0.22596542558768243</v>
+      </c>
+      <c r="C8">
+        <v>0.202703773668297</v>
+      </c>
+      <c r="D8">
+        <v>0.18146066004951675</v>
+      </c>
+      <c r="E8">
+        <v>0.16845661989366126</v>
+      </c>
+      <c r="F8">
+        <v>0.11678987307369015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>0.23276768432963732</v>
+      </c>
+      <c r="B9">
+        <v>0.22329207475776353</v>
+      </c>
+      <c r="C9">
+        <v>0.19663799959953079</v>
+      </c>
+      <c r="D9">
+        <v>0.17279191160023272</v>
+      </c>
+      <c r="E9">
+        <v>0.15848407315701624</v>
+      </c>
+      <c r="F9">
+        <v>0.10439494052893267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>0.23139844434258416</v>
+      </c>
+      <c r="B10">
+        <v>0.22064399254252082</v>
+      </c>
+      <c r="C10">
+        <v>0.1907421179707893</v>
+      </c>
+      <c r="D10">
+        <v>0.16456086243211812</v>
+      </c>
+      <c r="E10">
+        <v>0.14917704036336582</v>
+      </c>
+      <c r="F10">
+        <v>9.3796722981055E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>0.23003530728721144</v>
+      </c>
+      <c r="B11">
+        <v>0.21802143493755069</v>
+      </c>
+      <c r="C11">
+        <v>0.18501721631430007</v>
+      </c>
+      <c r="D11">
+        <v>0.15676106311135191</v>
+      </c>
+      <c r="E11">
+        <v>0.14051217886912468</v>
+      </c>
+      <c r="F11">
+        <v>8.4720552415379E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0.22867831123726023</v>
+      </c>
+      <c r="B12">
+        <v>0.21542464145089724</v>
+      </c>
+      <c r="C12">
+        <v>0.1794637189063516</v>
+      </c>
+      <c r="D12">
+        <v>0.14938284387826717</v>
+      </c>
+      <c r="E12">
+        <v>0.13246078088644664</v>
+      </c>
+      <c r="F12">
+        <v>7.6922979976319306E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>0.22732749332153174</v>
+      </c>
+      <c r="B13">
+        <v>0.21285383480606401</v>
+      </c>
+      <c r="C13">
+        <v>0.17408141283901166</v>
+      </c>
+      <c r="D13">
+        <v>0.14241384750356204</v>
+      </c>
+      <c r="E13">
+        <v>0.12499037939225566</v>
+      </c>
+      <c r="F13">
+        <v>7.0195330732966341E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>0.22598288970888195</v>
+      </c>
+      <c r="B14">
+        <v>0.2103092206977262</v>
+      </c>
+      <c r="C14">
+        <v>0.16886948205556535</v>
+      </c>
+      <c r="D14">
+        <v>0.13583957209470698</v>
+      </c>
+      <c r="E14">
+        <v>0.11806619845238855</v>
+      </c>
+      <c r="F14">
+        <v>6.4362398142722599E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>0.22464453559401529</v>
+      </c>
+      <c r="B15">
+        <v>0.20779098759982209</v>
+      </c>
+      <c r="C15">
+        <v>0.1638265478102261</v>
+      </c>
+      <c r="D15">
+        <v>0.12964389584905217</v>
+      </c>
+      <c r="E15">
+        <v>0.11165239177027833</v>
+      </c>
+      <c r="F15">
+        <v>5.9278852389163084E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>0.22331246518408293</v>
+      </c>
+      <c r="B16">
+        <v>0.2052993066254179</v>
+      </c>
+      <c r="C16">
+        <v>0.15895071400404875</v>
+      </c>
+      <c r="D16">
+        <v>0.12380956324187031</v>
+      </c>
+      <c r="E16">
+        <v>0.10571304830180256</v>
+      </c>
+      <c r="F16">
+        <v>5.482491027939574E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>0.22198671168609313</v>
+      </c>
+      <c r="B17">
+        <v>0.20283433143747986</v>
+      </c>
+      <c r="C17">
+        <v>0.1542396159006717</v>
+      </c>
+      <c r="D17">
+        <v>0.11831861932755905</v>
+      </c>
+      <c r="E17">
+        <v>0.10021296930959503</v>
+      </c>
+      <c r="F17">
+        <v>5.0902083513451699E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>0.22066730729513706</v>
+      </c>
+      <c r="B18">
+        <v>0.20039619820943533</v>
+      </c>
+      <c r="C18">
+        <v>0.14969047082553455</v>
+      </c>
+      <c r="D18">
+        <v>0.11315278510804333</v>
+      </c>
+      <c r="E18">
+        <v>9.5118237483910822E-2</v>
+      </c>
+      <c r="F18">
+        <v>4.7429372470245534E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>0.21935428318343375</v>
+      </c>
+      <c r="B19">
+        <v>0.19798502563417694</v>
+      </c>
+      <c r="C19">
+        <v>0.14530012958791491</v>
+      </c>
+      <c r="D19">
+        <v>0.10829377197312121</v>
+      </c>
+      <c r="E19">
+        <v>9.0396607278370303E-2</v>
+      </c>
+      <c r="F19">
+        <v>4.4340023833243224E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>0.21804766949019649</v>
+      </c>
+      <c r="B20">
+        <v>0.19560091497995413</v>
+      </c>
+      <c r="C20">
+        <v>0.1410651275242675</v>
+      </c>
+      <c r="D20">
+        <v>0.10372353697020928</v>
+      </c>
+      <c r="E20">
+        <v>8.6017748415939219E-2</v>
+      </c>
+      <c r="F20">
+        <v>4.1578846221857452E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0.21674749531232129</v>
+      </c>
+      <c r="B21">
+        <v>0.19324395019140397</v>
+      </c>
+      <c r="C21">
+        <v>0.13698173423274129</v>
+      </c>
+      <c r="D21">
+        <v>9.9424483204908459E-2</v>
+      </c>
+      <c r="E21">
+        <v>8.1953373559056492E-2</v>
+      </c>
+      <c r="F21">
+        <v>3.9100024391086813E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>0.21545378869589749</v>
+      </c>
+      <c r="B22">
+        <v>0.19091419803380841</v>
+      </c>
+      <c r="C22">
+        <v>0.13304600124279031</v>
+      </c>
+      <c r="D22">
+        <v>9.5379611189992164E-2</v>
+      </c>
+      <c r="E22">
+        <v>7.8177278008739776E-2</v>
+      </c>
+      <c r="F22">
+        <v>3.6865355889397926E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>0.214166576628539</v>
+      </c>
+      <c r="B23">
+        <v>0.18861170827851184</v>
+      </c>
+      <c r="C23">
+        <v>0.12925380703270212</v>
+      </c>
+      <c r="D23">
+        <v>9.1572627665928302E-2</v>
+      </c>
+      <c r="E23">
+        <v>7.4665315176863534E-2</v>
+      </c>
+      <c r="F23">
+        <v>3.4842835087706754E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>0.21288588503253308</v>
+      </c>
+      <c r="B24">
+        <v>0.18633651392731257</v>
+      </c>
+      <c r="C24">
+        <v>0.12560089896573273</v>
+      </c>
+      <c r="D24">
+        <v>8.7988018525968686E-2</v>
+      </c>
+      <c r="E24">
+        <v>7.1395327245311377E-2</v>
+      </c>
+      <c r="F24">
+        <v>3.3005517883895677E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>0.21161173875880418</v>
+      </c>
+      <c r="B25">
+        <v>0.18408863147353058</v>
+      </c>
+      <c r="C25">
+        <v>0.12208293185828389</v>
+      </c>
+      <c r="D25">
+        <v>8.4611092183809494E-2</v>
+      </c>
+      <c r="E25">
+        <v>6.8347046350994312E-2</v>
+      </c>
+      <c r="F25">
+        <v>3.1330610940849574E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>0.21034416158168673</v>
+      </c>
+      <c r="B26">
+        <v>0.18186806119737448</v>
+      </c>
+      <c r="C26">
+        <v>0.11869550301870918</v>
+      </c>
+      <c r="D26">
+        <v>8.1427999177807187E-2</v>
+      </c>
+      <c r="E26">
+        <v>6.5501978053987955E-2</v>
+      </c>
+      <c r="F26">
+        <v>2.9798739612585584E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>0.20908317619450248</v>
+      </c>
+      <c r="B27">
+        <v>0.17967478749316157</v>
+      </c>
+      <c r="C27">
+        <v>0.11543418370179451</v>
+      </c>
+      <c r="D27">
+        <v>7.842573313212739E-2</v>
+      </c>
+      <c r="E27">
+        <v>6.2843275843365728E-2</v>
+      </c>
+      <c r="F27">
+        <v>2.839335778028651E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>0.20782880420593419</v>
+      </c>
+      <c r="B28">
+        <v>0.17750877922590497</v>
+      </c>
+      <c r="C28">
+        <v>0.11229454701173039</v>
+      </c>
+      <c r="D28">
+        <v>7.5592117477869716E-2</v>
+      </c>
+      <c r="E28">
+        <v>6.0355613006611825E-2</v>
+      </c>
+      <c r="F28">
+        <v>2.7100270395771342E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>0.20658106613718943</v>
+      </c>
+      <c r="B29">
+        <v>0.17536999011475216</v>
+      </c>
+      <c r="C29">
+        <v>0.10927219235630757</v>
+      </c>
+      <c r="D29">
+        <v>7.2915781633847751E-2</v>
+      </c>
+      <c r="E29">
+        <v>5.8025056280016044E-2</v>
+      </c>
+      <c r="F29">
+        <v>2.5907245673564741E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>0.2053399814199442</v>
+      </c>
+      <c r="B30">
+        <v>0.17325835914075249</v>
+      </c>
+      <c r="C30">
+        <v>0.10636276660852687</v>
+      </c>
+      <c r="D30">
+        <v>7.0386129692918964E-2</v>
+      </c>
+      <c r="E30">
+        <v>5.5838944234455193E-2</v>
+      </c>
+      <c r="F30">
+        <v>2.4803698768155375E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>0.20410556839505828</v>
+      </c>
+      <c r="B31">
+        <v>0.1711738109764416</v>
+      </c>
+      <c r="C31">
+        <v>0.10356198217058328</v>
+      </c>
+      <c r="D31">
+        <v>6.7993304074767918E-2</v>
+      </c>
+      <c r="E31">
+        <v>5.3785772254578659E-2</v>
+      </c>
+      <c r="F31">
+        <v>2.3780432633831283E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>0.20287784431205044</v>
+      </c>
+      <c r="B32">
+        <v>0.16911625643474981</v>
+      </c>
+      <c r="C32">
+        <v>0.1008656321612144</v>
+      </c>
+      <c r="D32">
+        <v>6.5728146097571216E-2</v>
+      </c>
+      <c r="E32">
+        <v>5.1855085165816155E-2</v>
+      </c>
+      <c r="F32">
+        <v>2.282942479195206E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>0.20165682532932294</v>
+      </c>
+      <c r="B33">
+        <v>0.16708559293478628</v>
+      </c>
+      <c r="C33">
+        <v>9.8269602962661323E-2</v>
+      </c>
+      <c r="D33">
+        <v>6.3582154989145684E-2</v>
+      </c>
+      <c r="E33">
+        <v>5.0037377988297521E-2</v>
+      </c>
+      <c r="F33">
+        <v>2.1943651098189226E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>0.20044252651512373</v>
+      </c>
+      <c r="B34">
+        <v>0.16508170498209707</v>
+      </c>
+      <c r="C34">
+        <v>9.5769884369911337E-2</v>
+      </c>
+      <c r="D34">
+        <v>6.1547446498459911E-2</v>
+      </c>
+      <c r="E34">
+        <v>4.8324004895857309E-2</v>
+      </c>
+      <c r="F34">
+        <v>2.1116939452806287E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>